<commit_message>
Movie directory auto-fill in feature
</commit_message>
<xml_diff>
--- a/src/test/resources/movies.xlsx
+++ b/src/test/resources/movies.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Moviebase" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>8 1/2</t>
   </si>
   <si>
-    <t>A clockwork orange</t>
-  </si>
-  <si>
     <t>Stanley Kubrik</t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t>Moet nog bekijken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: clockwork     orange  </t>
   </si>
 </sst>
 </file>
@@ -351,8 +351,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -397,7 +397,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -408,8 +408,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -704,88 +704,88 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="75.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="20.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="75.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="20.81640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="5" customWidth="1"/>
     <col min="13" max="13" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" customWidth="1"/>
+    <col min="14" max="14" width="25.26953125" customWidth="1"/>
+    <col min="15" max="15" width="25.81640625" customWidth="1"/>
+    <col min="16" max="16" width="28.81640625" customWidth="1"/>
     <col min="17" max="17" width="29" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="R1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -793,19 +793,19 @@
         <v>2012</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I2" s="2">
         <v>15.2</v>
@@ -820,19 +820,19 @@
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -840,98 +840,98 @@
         <v>1963</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3"/>
       <c r="Q3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B4">
         <v>1971</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L4" s="5">
         <v>7.5</v>
       </c>
       <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="5">
         <v>9</v>
       </c>
       <c r="M5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6">
         <v>2019</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L6" s="5">
         <v>9</v>
       </c>
       <c r="M6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -949,250 +949,250 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="30" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvement of the crosscheck, testing, folder option
</commit_message>
<xml_diff>
--- a/src/test/resources/movies.xlsx
+++ b/src/test/resources/movies.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Moviebase" sheetId="1" r:id="rId1"/>
     <sheet name="Genres" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$S$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$T$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>Rating</t>
   </si>
@@ -344,6 +344,24 @@
   </si>
   <si>
     <t xml:space="preserve">A: clockwork     orange  </t>
+  </si>
+  <si>
+    <t>The Great Dictator</t>
+  </si>
+  <si>
+    <t>comedy/_Charlie Chaplin</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>The Great Dictator (1941)</t>
+  </si>
+  <si>
+    <t>Bohemian Rhapsody</t>
+  </si>
+  <si>
+    <t>Bohemian Rhapsody (2018)</t>
   </si>
 </sst>
 </file>
@@ -351,8 +369,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -397,7 +415,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -408,8 +426,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -698,35 +716,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="75.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="20.81640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="20.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="5" customWidth="1"/>
     <col min="13" max="13" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.26953125" customWidth="1"/>
-    <col min="15" max="15" width="25.81640625" customWidth="1"/>
-    <col min="16" max="16" width="28.81640625" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="28.85546875" customWidth="1"/>
     <col min="17" max="17" width="29" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -784,8 +802,11 @@
       <c r="S1" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="T1" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -832,7 +853,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -842,7 +863,6 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
@@ -857,7 +877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>103</v>
       </c>
@@ -867,7 +887,6 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
@@ -887,7 +906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -897,7 +916,6 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
@@ -914,28 +932,57 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6">
+        <v>2018</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2019</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L7" s="5">
         <v>9</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8">
+        <v>1941</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:S6"/>
+  <autoFilter ref="A1:T8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -949,13 +996,13 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -963,7 +1010,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
@@ -971,7 +1018,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -979,7 +1026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -987,7 +1034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -995,7 +1042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1003,7 +1050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1066,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1027,7 +1074,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1035,7 +1082,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1090,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1098,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1059,7 +1106,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1067,7 +1114,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1122,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1083,7 +1130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1091,7 +1138,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1099,7 +1146,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1107,7 +1154,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1115,7 +1162,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1123,7 +1170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1131,7 +1178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1139,7 +1186,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1147,7 +1194,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1155,7 +1202,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1163,7 +1210,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1171,7 +1218,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1179,7 +1226,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1187,7 +1234,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Change of column, test adaptation
</commit_message>
<xml_diff>
--- a/src/test/resources/movies.xlsx
+++ b/src/test/resources/movies.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Moviebase" sheetId="1" r:id="rId1"/>
     <sheet name="Genres" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$T$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Moviebase!$A$1:$T$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="111">
   <si>
     <t>Rating</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Bohemian Rhapsody (2018)</t>
+  </si>
+  <si>
+    <t>Check!</t>
   </si>
 </sst>
 </file>
@@ -369,8 +372,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -415,7 +418,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -426,8 +429,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -722,29 +725,29 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="20.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="50" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" customWidth="1"/>
-    <col min="17" max="17" width="29" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="20.81640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="50" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.26953125" customWidth="1"/>
+    <col min="16" max="16" width="25.81640625" customWidth="1"/>
+    <col min="17" max="17" width="28.81640625" customWidth="1"/>
+    <col min="18" max="18" width="29" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -758,55 +761,55 @@
         <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -819,41 +822,41 @@
       <c r="D2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>15.2</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>12.5</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>3</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>100</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -863,21 +866,21 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M3"/>
-      <c r="Q3" t="s">
+      <c r="N3"/>
+      <c r="R3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>103</v>
       </c>
@@ -887,26 +890,26 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>7.5</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,23 +919,23 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>9</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>108</v>
       </c>
@@ -945,9 +948,9 @@
       <c r="D6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>91</v>
       </c>
@@ -960,14 +963,14 @@
       <c r="D7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>9</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>104</v>
       </c>
@@ -979,6 +982,9 @@
       </c>
       <c r="D8" s="2" t="s">
         <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -996,13 +1002,13 @@
       <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>75</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>

</xml_diff>